<commit_message>
Rigged default humanoid model
</commit_message>
<xml_diff>
--- a/MAG production/Template - Shot checklist.xlsx
+++ b/MAG production/Template - Shot checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://morrisville-my.sharepoint.com/personal/fowler086_morrisville_edu/Documents/Documents/GitHub/MAG-common-files/MAG production/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{FA50C2F6-2EB5-4EFE-B5BE-4BAABBA45DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CC65C54-BCF9-4710-A969-489ABCC4FECD}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{FA50C2F6-2EB5-4EFE-B5BE-4BAABBA45DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12777574-E10E-4BAC-9FC4-70F787A11937}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="23232" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,16 +30,16 @@
     <t>Green = Complete | Yellow = In progress | Red = No progress</t>
   </si>
   <si>
-    <t>Shot number</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
     <t>Status</t>
   </si>
   <si>
-    <t>Deadlines</t>
+    <t>Shot Number</t>
+  </si>
+  <si>
+    <t>Task Number</t>
   </si>
 </sst>
 </file>
@@ -382,50 +382,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="1" max="1" width="55.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.77734375" customWidth="1"/>
     <col min="8" max="8" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>1</v>
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>2</v>
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>3</v>
       </c>

</xml_diff>